<commit_message>
Update fix error log
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/input/input.xlsx
+++ b/Netbeans/ANA-ADDIX/input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E24F50-7272-452A-95E3-CA4BB12A86F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE76EE51-7AE4-4AD4-B987-6046C7E277E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
-    <t>techable</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>URL</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -138,21 +134,6 @@
     <t>?s=</t>
   </si>
   <si>
-    <t>body &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; section &gt; a</t>
-  </si>
-  <si>
-    <t>body &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; section &gt; a&gt;div&gt;div&gt;h3</t>
-  </si>
-  <si>
-    <t>body &gt; div &gt; div &gt; div&gt; div &gt; div &gt; div&gt; time</t>
-  </si>
-  <si>
-    <t>body &gt; div &gt; div  div &gt; div &gt; div.te-cms-body</t>
-  </si>
-  <si>
-    <t>https://techable.jp</t>
-  </si>
-  <si>
     <t>click_Search</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -162,13 +143,6 @@
   </si>
   <si>
     <t>Domain</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>14件</t>
-    <rPh sb="2" eb="3">
-      <t>ケン</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -188,10 +162,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://techable.jp/page/(pagenum)/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>CrawlSwitch</t>
   </si>
   <si>
@@ -210,10 +180,39 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>body &gt; div.te-viewport &gt; div.te-contents &gt; div.te-layout &gt; div.te-layout__col.te-layout__col--main &gt; div &gt; div.paging &gt; div &gt; a</t>
-  </si>
-  <si>
     <t>Item pages element</t>
+  </si>
+  <si>
+    <t>ainow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://ainow.ai/?s=(keyword)</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; a</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; a &gt; section &gt; h1</t>
+  </si>
+  <si>
+    <t>#main &gt; article &gt; header &gt; p &gt; time</t>
+  </si>
+  <si>
+    <t>#main &gt; article &gt; section</t>
+  </si>
+  <si>
+    <t>https://ainow.ai</t>
+  </si>
+  <si>
+    <t>#main &gt; nav &gt; ul &gt; li</t>
+  </si>
+  <si>
+    <t>20件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -305,13 +304,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -612,7 +632,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -631,84 +651,84 @@
     <col min="15" max="15" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="9" style="2"/>
     <col min="20" max="20" width="38.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
         <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -717,56 +737,56 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="M2" s="4">
         <v>2</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="Q2" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S2" s="4">
         <v>0</v>
       </c>
       <c r="T2" s="4"/>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>42</v>
+      <c r="V2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -803,97 +823,97 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update library jsoup error
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/input/input.xlsx
+++ b/Netbeans/ANA-ADDIX/input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE76EE51-7AE4-4AD4-B987-6046C7E277E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1143CE-9676-4950-A24E-FE8D6CC56355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,12 +128,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>page/</t>
-  </si>
-  <si>
-    <t>?s=</t>
-  </si>
-  <si>
     <t>click_Search</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -183,32 +177,37 @@
     <t>Item pages element</t>
   </si>
   <si>
-    <t>ainow</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://ainow.ai/?s=(keyword)</t>
-  </si>
-  <si>
-    <t>#main &gt; div &gt; article &gt; a</t>
-  </si>
-  <si>
-    <t>#main &gt; div &gt; article &gt; a &gt; section &gt; h1</t>
-  </si>
-  <si>
-    <t>#main &gt; article &gt; header &gt; p &gt; time</t>
-  </si>
-  <si>
-    <t>#main &gt; article &gt; section</t>
-  </si>
-  <si>
-    <t>https://ainow.ai</t>
-  </si>
-  <si>
-    <t>#main &gt; nav &gt; ul &gt; li</t>
-  </si>
-  <si>
-    <t>20件</t>
+    <t>kyodonews</t>
+  </si>
+  <si>
+    <t>https://kyodonewsprwire.jp/search?s=(keyword)</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div &gt; div &gt; h4 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; p.releae-up-date</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div.release-body &gt; p:last-child</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div.release-body &gt; p</t>
+  </si>
+  <si>
+    <t>&amp;page=</t>
+  </si>
+  <si>
+    <t>https://kyodonewsprwire.jp</t>
+  </si>
+  <si>
+    <t>stp=1</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div.col-md-12.col-lg-9.search-area &gt; div.col-md-12 &gt; ul &gt; li &gt; a</t>
+  </si>
+  <si>
+    <t>25件</t>
     <rPh sb="2" eb="3">
       <t>ケン</t>
     </rPh>
@@ -632,7 +631,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -660,19 +659,19 @@
         <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -693,13 +692,13 @@
         <v>24</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>25</v>
@@ -717,18 +716,18 @@
         <v>29</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:22" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -743,37 +742,37 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="M2" s="4">
         <v>2</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="Q2" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>30</v>
@@ -823,7 +822,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
Testing redownload & backup
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/input/input.xlsx
+++ b/Netbeans/ANA-ADDIX/input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254A6C09-0D97-4ACD-9CB5-124E4ED167DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA39D28-0839-47DC-B997-7AEED17AEFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="console" sheetId="3" r:id="rId1"/>
@@ -1072,7 +1072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1093,6 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1402,9 +1403,9 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1463,22 +1464,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="36.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="36.5546875" style="1" customWidth="1"/>
     <col min="10" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="9" style="1"/>
-    <col min="22" max="23" width="20.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="20.109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.109375" style="1" customWidth="1"/>
     <col min="25" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2464,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="11">
         <v>0</v>
@@ -2938,7 +2939,7 @@
       <c r="H20" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="16" t="s">
         <v>27</v>
       </c>
       <c r="J20" s="3" t="s">
@@ -3068,7 +3069,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="11">
         <v>0</v>
@@ -3406,9 +3407,10 @@
     <hyperlink ref="I22" r:id="rId8" xr:uid="{262EAE78-373E-4BAD-8A14-59EACC50C8C8}"/>
     <hyperlink ref="I19" r:id="rId9" xr:uid="{2CCFBAD4-10C3-4804-8767-4F484644E814}"/>
     <hyperlink ref="I14" r:id="rId10" xr:uid="{D4AA9688-133A-41DA-A1B3-1DC21E360282}"/>
+    <hyperlink ref="I20" r:id="rId11" xr:uid="{D9B45338-918F-43DA-859C-EDCAC7D3F5E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -3418,13 +3420,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -3442,7 +3444,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3450,7 +3452,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3596,7 +3598,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">

</xml_diff>